<commit_message>
Added date time values and hashes to data dictionary
</commit_message>
<xml_diff>
--- a/doc/data_dictionary.xlsx
+++ b/doc/data_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\CzechTutor\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F8AE7A-49E5-4010-9C85-3F0189F50B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9A4403-A13C-4B96-88C9-72BCD288C661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{A03E13AB-CF66-429B-A912-33A5021197AB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A03E13AB-CF66-429B-A912-33A5021197AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Lessons" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="78">
   <si>
     <t>Column Name</t>
   </si>
@@ -244,6 +244,36 @@
   </si>
   <si>
     <t>The lesson score.</t>
+  </si>
+  <si>
+    <t>date_time</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>2025-06-14 22:27:18.182458</t>
+  </si>
+  <si>
+    <t>date_time_hash</t>
+  </si>
+  <si>
+    <t>op8+4WOsllnwVsSOdtC7Jg==</t>
+  </si>
+  <si>
+    <t>An MD5 hash of the date time value.</t>
+  </si>
+  <si>
+    <t>The date time the lesson was created.</t>
+  </si>
+  <si>
+    <t>The date time the question was created.</t>
+  </si>
+  <si>
+    <t>The date time the answer was created.</t>
+  </si>
+  <si>
+    <t>The date time the result was created.</t>
   </si>
 </sst>
 </file>
@@ -287,9 +317,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1CC80A8-D8B0-4010-A2EC-A9DBB086E33B}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -758,6 +789,40 @@
         <v>22</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -765,10 +830,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{056DD76E-8279-4312-844A-D48A505E9857}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -938,6 +1003,40 @@
         <v>42</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -946,10 +1045,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED906043-1473-403D-A682-3AB02926B866}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1063,6 +1162,40 @@
         <v>59</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1070,10 +1203,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAE73DF7-0A78-4B0F-9587-BF21DDDF2261}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1170,6 +1303,40 @@
         <v>67</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1179,8 +1346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B40765BD-8F70-4ED7-9C66-9960F4EE9B60}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>